<commit_message>
version with dual gmt tx
</commit_message>
<xml_diff>
--- a/examples/EMTF_MPCX_full/src/link_map_MPCX_CPPF_GE11.xlsx
+++ b/examples/EMTF_MPCX_full/src/link_map_MPCX_CPPF_GE11.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="75">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -546,10 +546,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M69"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M27" activeCellId="0" sqref="M27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C68" activeCellId="0" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2301,28 +2301,54 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B69" s="3" t="n">
+      <c r="B69" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D69" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E69" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F69" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G69" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H69" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C69" s="3" t="n">
+      <c r="C70" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D70" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E69" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F69" s="3" t="n">
+      <c r="E70" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F70" s="3" t="n">
         <v>125</v>
       </c>
-      <c r="G69" s="3" t="s">
+      <c r="G70" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H69" s="3" t="n">
+      <c r="H70" s="3" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding OMTF MPCX setup
</commit_message>
<xml_diff>
--- a/examples/EMTF_MPCX_full/src/link_map_MPCX_CPPF_GE11.xlsx
+++ b/examples/EMTF_MPCX_full/src/link_map_MPCX_CPPF_GE11.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="74">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -146,9 +146,6 @@
   </si>
   <si>
     <t xml:space="preserve">28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$</t>
   </si>
   <si>
     <t xml:space="preserve">27</t>
@@ -546,10 +543,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C68" activeCellId="0" sqref="C68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M27" activeCellId="0" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1230,9 +1227,6 @@
       <c r="H27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="M27" s="0" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
@@ -1242,7 +1236,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>17</v>
@@ -1268,19 +1262,19 @@
         <v>15</v>
       </c>
       <c r="C29" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>44</v>
       </c>
       <c r="H29" s="13" t="s">
         <v>21</v>
@@ -1294,7 +1288,7 @@
         <v>15</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>17</v>
@@ -1306,7 +1300,7 @@
         <v>19</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H30" s="13" t="s">
         <v>15</v>
@@ -1332,7 +1326,7 @@
         <v>19</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H31" s="13" t="s">
         <v>24</v>
@@ -1346,7 +1340,7 @@
         <v>21</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>17</v>
@@ -1358,7 +1352,7 @@
         <v>19</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H32" s="13" t="s">
         <v>26</v>
@@ -1372,7 +1366,7 @@
         <v>15</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>17</v>
@@ -1384,7 +1378,7 @@
         <v>19</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H33" s="13" t="s">
         <v>27</v>
@@ -1398,7 +1392,7 @@
         <v>15</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>17</v>
@@ -1410,7 +1404,7 @@
         <v>19</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H34" s="13" t="s">
         <v>29</v>
@@ -1424,7 +1418,7 @@
         <v>21</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>17</v>
@@ -1436,7 +1430,7 @@
         <v>19</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H35" s="13" t="s">
         <v>30</v>
@@ -1450,7 +1444,7 @@
         <v>21</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>17</v>
@@ -1462,7 +1456,7 @@
         <v>19</v>
       </c>
       <c r="G36" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H36" s="13" t="s">
         <v>32</v>
@@ -1476,19 +1470,19 @@
         <v>15</v>
       </c>
       <c r="C37" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="18" t="s">
         <v>48</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>49</v>
       </c>
       <c r="H37" s="17" t="s">
         <v>21</v>
@@ -1502,7 +1496,7 @@
         <v>15</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>17</v>
@@ -1514,7 +1508,7 @@
         <v>19</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H38" s="17" t="s">
         <v>15</v>
@@ -1528,7 +1522,7 @@
         <v>21</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>17</v>
@@ -1540,7 +1534,7 @@
         <v>19</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H39" s="17" t="s">
         <v>24</v>
@@ -1554,7 +1548,7 @@
         <v>21</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>17</v>
@@ -1566,7 +1560,7 @@
         <v>19</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H40" s="17" t="s">
         <v>26</v>
@@ -1580,7 +1574,7 @@
         <v>15</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>17</v>
@@ -1592,7 +1586,7 @@
         <v>19</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H41" s="17" t="s">
         <v>27</v>
@@ -1606,7 +1600,7 @@
         <v>15</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>17</v>
@@ -1618,7 +1612,7 @@
         <v>19</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H42" s="17" t="s">
         <v>29</v>
@@ -1632,7 +1626,7 @@
         <v>21</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>17</v>
@@ -1644,7 +1638,7 @@
         <v>19</v>
       </c>
       <c r="G43" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H43" s="17" t="s">
         <v>30</v>
@@ -1658,7 +1652,7 @@
         <v>21</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D44" s="18" t="s">
         <v>17</v>
@@ -1670,7 +1664,7 @@
         <v>19</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H44" s="17" t="s">
         <v>32</v>
@@ -1684,19 +1678,19 @@
         <v>15</v>
       </c>
       <c r="C45" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="E45" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="F45" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F45" s="13" t="s">
+      <c r="G45" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="G45" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="H45" s="13" t="s">
         <v>30</v>
@@ -1710,19 +1704,19 @@
         <v>15</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D46" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="F46" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F46" s="13" t="s">
+      <c r="G46" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="G46" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="H46" s="13" t="s">
         <v>29</v>
@@ -1736,19 +1730,19 @@
         <v>21</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D47" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E47" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="F47" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F47" s="13" t="s">
+      <c r="G47" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="G47" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="H47" s="13" t="s">
         <v>21</v>
@@ -1762,19 +1756,19 @@
         <v>21</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D48" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E48" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="F48" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F48" s="13" t="s">
+      <c r="G48" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="G48" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="H48" s="13" t="s">
         <v>15</v>
@@ -1788,19 +1782,19 @@
         <v>15</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D49" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E49" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E49" s="14" t="s">
+      <c r="F49" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F49" s="13" t="s">
+      <c r="G49" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="G49" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="H49" s="13" t="s">
         <v>26</v>
@@ -1814,19 +1808,19 @@
         <v>15</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D50" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E50" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="F50" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F50" s="13" t="s">
+      <c r="G50" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="G50" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="H50" s="13" t="s">
         <v>27</v>
@@ -1840,19 +1834,19 @@
         <v>21</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D51" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E51" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="F51" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F51" s="13" t="s">
+      <c r="G51" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="G51" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="H51" s="13" t="s">
         <v>24</v>
@@ -1866,19 +1860,19 @@
         <v>15</v>
       </c>
       <c r="C52" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G52" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F52" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G52" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="H52" s="9" t="s">
         <v>21</v>
@@ -1892,7 +1886,7 @@
         <v>15</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D53" s="10" t="s">
         <v>17</v>
@@ -1904,7 +1898,7 @@
         <v>19</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H53" s="9" t="s">
         <v>15</v>
@@ -1918,19 +1912,19 @@
         <v>21</v>
       </c>
       <c r="C54" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="H54" s="9" t="s">
         <v>24</v>
@@ -1944,7 +1938,7 @@
         <v>21</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D55" s="10" t="s">
         <v>17</v>
@@ -1956,7 +1950,7 @@
         <v>19</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H55" s="9" t="s">
         <v>26</v>
@@ -1970,7 +1964,7 @@
         <v>15</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D56" s="10" t="s">
         <v>17</v>
@@ -1982,7 +1976,7 @@
         <v>19</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H56" s="9" t="s">
         <v>27</v>
@@ -1996,7 +1990,7 @@
         <v>15</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D57" s="10" t="s">
         <v>17</v>
@@ -2008,7 +2002,7 @@
         <v>19</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H57" s="9" t="s">
         <v>29</v>
@@ -2022,7 +2016,7 @@
         <v>21</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D58" s="10" t="s">
         <v>17</v>
@@ -2034,7 +2028,7 @@
         <v>19</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>30</v>
@@ -2048,7 +2042,7 @@
         <v>21</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D59" s="10" t="s">
         <v>17</v>
@@ -2060,7 +2054,7 @@
         <v>19</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H59" s="9" t="s">
         <v>32</v>
@@ -2074,22 +2068,22 @@
         <v>15</v>
       </c>
       <c r="C60" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H60" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G60" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="H60" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2100,19 +2094,19 @@
         <v>15</v>
       </c>
       <c r="C61" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D61" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D61" s="19" t="s">
+      <c r="E61" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61" s="19" t="s">
         <v>69</v>
-      </c>
-      <c r="E61" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F61" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G61" s="19" t="s">
-        <v>70</v>
       </c>
       <c r="H61" s="19" t="s">
         <v>21</v>
@@ -2126,19 +2120,19 @@
         <v>15</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D62" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F62" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G62" s="19" t="s">
         <v>69</v>
-      </c>
-      <c r="E62" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F62" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G62" s="19" t="s">
-        <v>70</v>
       </c>
       <c r="H62" s="19" t="s">
         <v>15</v>
@@ -2152,19 +2146,19 @@
         <v>21</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D63" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F63" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G63" s="19" t="s">
         <v>69</v>
-      </c>
-      <c r="E63" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F63" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G63" s="19" t="s">
-        <v>70</v>
       </c>
       <c r="H63" s="19" t="s">
         <v>24</v>
@@ -2178,19 +2172,19 @@
         <v>21</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D64" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G64" s="19" t="s">
         <v>69</v>
-      </c>
-      <c r="E64" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F64" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G64" s="19" t="s">
-        <v>70</v>
       </c>
       <c r="H64" s="19" t="s">
         <v>26</v>
@@ -2207,16 +2201,16 @@
         <v>32</v>
       </c>
       <c r="D65" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F65" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G65" s="19" t="s">
         <v>69</v>
-      </c>
-      <c r="E65" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F65" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G65" s="19" t="s">
-        <v>70</v>
       </c>
       <c r="H65" s="19" t="s">
         <v>27</v>
@@ -2233,16 +2227,16 @@
         <v>30</v>
       </c>
       <c r="D66" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G66" s="19" t="s">
         <v>69</v>
-      </c>
-      <c r="E66" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F66" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G66" s="19" t="s">
-        <v>70</v>
       </c>
       <c r="H66" s="19" t="s">
         <v>29</v>
@@ -2259,16 +2253,16 @@
         <v>30</v>
       </c>
       <c r="D67" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F67" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G67" s="19" t="s">
         <v>69</v>
-      </c>
-      <c r="E67" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F67" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G67" s="19" t="s">
-        <v>70</v>
       </c>
       <c r="H67" s="19" t="s">
         <v>30</v>
@@ -2276,7 +2270,7 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B68" s="22" t="s">
         <v>21</v>
@@ -2285,16 +2279,16 @@
         <v>37</v>
       </c>
       <c r="D68" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E68" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E68" s="21" t="s">
+      <c r="F68" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F68" s="22" t="s">
-        <v>56</v>
-      </c>
       <c r="G68" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H68" s="22" t="s">
         <v>21</v>
@@ -2302,7 +2296,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69" s="22" t="s">
         <v>15</v>
@@ -2311,16 +2305,16 @@
         <v>28</v>
       </c>
       <c r="D69" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E69" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E69" s="21" t="s">
+      <c r="F69" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F69" s="22" t="s">
-        <v>56</v>
-      </c>
       <c r="G69" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H69" s="22" t="s">
         <v>15</v>
@@ -2328,7 +2322,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B70" s="3" t="n">
         <v>1</v>
@@ -2337,7 +2331,7 @@
         <v>4</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>18</v>
@@ -2346,7 +2340,7 @@
         <v>125</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H70" s="3" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
corrected refclk placement, LHC clock was incorrectly placed as refclk
</commit_message>
<xml_diff>
--- a/examples/EMTF_MPCX_full/src/link_map_MPCX_CPPF_GE11.xlsx
+++ b/examples/EMTF_MPCX_full/src/link_map_MPCX_CPPF_GE11.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="75">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t xml:space="preserve">19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swatch index</t>
   </si>
   <si>
     <t xml:space="preserve">CPPF</t>
@@ -546,7 +549,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M27" activeCellId="0" sqref="M27"/>
+      <selection pane="topLeft" activeCell="I47" activeCellId="0" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1669,6 +1672,9 @@
       <c r="H44" s="17" t="s">
         <v>32</v>
       </c>
+      <c r="I44" s="0" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="14" t="s">
@@ -1681,20 +1687,23 @@
         <v>52</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H45" s="13" t="s">
         <v>30</v>
       </c>
+      <c r="I45" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="14" t="s">
@@ -1704,23 +1713,26 @@
         <v>15</v>
       </c>
       <c r="C46" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G46" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F46" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G46" s="14" t="s">
-        <v>56</v>
       </c>
       <c r="H46" s="13" t="s">
         <v>29</v>
       </c>
+      <c r="I46" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="14" t="s">
@@ -1733,19 +1745,22 @@
         <v>51</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H47" s="13" t="s">
         <v>21</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1756,22 +1771,25 @@
         <v>21</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H48" s="13" t="s">
         <v>15</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,23 +1800,26 @@
         <v>15</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G49" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H49" s="13" t="s">
         <v>26</v>
       </c>
+      <c r="I49" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="14" t="s">
@@ -1808,23 +1829,26 @@
         <v>15</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H50" s="13" t="s">
         <v>27</v>
       </c>
+      <c r="I50" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="14" t="s">
@@ -1834,23 +1858,26 @@
         <v>21</v>
       </c>
       <c r="C51" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G51" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E51" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F51" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G51" s="14" t="s">
-        <v>56</v>
       </c>
       <c r="H51" s="13" t="s">
         <v>24</v>
       </c>
+      <c r="I51" s="0" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
@@ -1860,7 +1887,7 @@
         <v>15</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D52" s="10" t="s">
         <v>17</v>
@@ -1872,7 +1899,7 @@
         <v>19</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H52" s="9" t="s">
         <v>21</v>
@@ -1886,19 +1913,19 @@
         <v>15</v>
       </c>
       <c r="C53" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="H53" s="9" t="s">
         <v>15</v>
@@ -1912,7 +1939,7 @@
         <v>21</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>17</v>
@@ -1924,7 +1951,7 @@
         <v>19</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H54" s="9" t="s">
         <v>24</v>
@@ -1938,19 +1965,19 @@
         <v>21</v>
       </c>
       <c r="C55" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G55" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="D55" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G55" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="H55" s="9" t="s">
         <v>26</v>
@@ -1964,7 +1991,7 @@
         <v>15</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D56" s="10" t="s">
         <v>17</v>
@@ -1976,7 +2003,7 @@
         <v>19</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H56" s="9" t="s">
         <v>27</v>
@@ -1990,7 +2017,7 @@
         <v>15</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D57" s="10" t="s">
         <v>17</v>
@@ -2002,7 +2029,7 @@
         <v>19</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H57" s="9" t="s">
         <v>29</v>
@@ -2016,7 +2043,7 @@
         <v>21</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D58" s="10" t="s">
         <v>17</v>
@@ -2028,7 +2055,7 @@
         <v>19</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>30</v>
@@ -2042,7 +2069,7 @@
         <v>21</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D59" s="10" t="s">
         <v>17</v>
@@ -2054,7 +2081,7 @@
         <v>19</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H59" s="9" t="s">
         <v>32</v>
@@ -2068,7 +2095,7 @@
         <v>15</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D60" s="10" t="s">
         <v>17</v>
@@ -2080,10 +2107,10 @@
         <v>19</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H60" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2094,19 +2121,19 @@
         <v>15</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D61" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F61" s="19" t="s">
         <v>19</v>
       </c>
       <c r="G61" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H61" s="19" t="s">
         <v>21</v>
@@ -2120,19 +2147,19 @@
         <v>15</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D62" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F62" s="19" t="s">
         <v>19</v>
       </c>
       <c r="G62" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H62" s="19" t="s">
         <v>15</v>
@@ -2146,19 +2173,19 @@
         <v>21</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D63" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F63" s="19" t="s">
         <v>19</v>
       </c>
       <c r="G63" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H63" s="19" t="s">
         <v>24</v>
@@ -2172,19 +2199,19 @@
         <v>21</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D64" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F64" s="19" t="s">
         <v>19</v>
       </c>
       <c r="G64" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H64" s="19" t="s">
         <v>26</v>
@@ -2201,16 +2228,16 @@
         <v>32</v>
       </c>
       <c r="D65" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E65" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F65" s="19" t="s">
         <v>19</v>
       </c>
       <c r="G65" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H65" s="19" t="s">
         <v>27</v>
@@ -2227,16 +2254,16 @@
         <v>30</v>
       </c>
       <c r="D66" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E66" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F66" s="19" t="s">
         <v>19</v>
       </c>
       <c r="G66" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H66" s="19" t="s">
         <v>29</v>
@@ -2253,16 +2280,16 @@
         <v>30</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E67" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F67" s="19" t="s">
         <v>19</v>
       </c>
       <c r="G67" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H67" s="19" t="s">
         <v>30</v>
@@ -2270,7 +2297,7 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B68" s="22" t="s">
         <v>21</v>
@@ -2279,16 +2306,16 @@
         <v>37</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E68" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F68" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G68" s="21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H68" s="22" t="s">
         <v>21</v>
@@ -2296,7 +2323,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B69" s="22" t="s">
         <v>15</v>
@@ -2305,16 +2332,16 @@
         <v>28</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E69" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F69" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G69" s="21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H69" s="22" t="s">
         <v>15</v>
@@ -2322,7 +2349,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B70" s="3" t="n">
         <v>1</v>
@@ -2331,7 +2358,7 @@
         <v>4</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>18</v>
@@ -2340,7 +2367,7 @@
         <v>125</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H70" s="3" t="n">
         <v>0</v>

</xml_diff>